<commit_message>
completion of paper draft
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="377">
   <si>
     <t>#GENERAL CHARACTERISTICS - "CGenerales"</t>
   </si>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H202" sqref="H202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3599,6 +3599,9 @@
       <c r="G168" t="s">
         <v>285</v>
       </c>
+      <c r="H168" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
@@ -3610,6 +3613,9 @@
       <c r="G169" t="s">
         <v>285</v>
       </c>
+      <c r="H169" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
@@ -3621,6 +3627,9 @@
       <c r="G170" t="s">
         <v>285</v>
       </c>
+      <c r="H170" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
@@ -3632,6 +3641,9 @@
       <c r="G171" t="s">
         <v>285</v>
       </c>
+      <c r="H171" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
@@ -3643,6 +3655,9 @@
       <c r="G172" t="s">
         <v>285</v>
       </c>
+      <c r="H172" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
@@ -3654,6 +3669,9 @@
       <c r="G173" t="s">
         <v>285</v>
       </c>
+      <c r="H173" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
@@ -3665,6 +3683,9 @@
       <c r="G174" t="s">
         <v>285</v>
       </c>
+      <c r="H174" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
@@ -3686,7 +3707,7 @@
         <v>376</v>
       </c>
       <c r="H175" t="s">
-        <v>376</v>
+        <v>285</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -3699,6 +3720,9 @@
       <c r="G176" t="s">
         <v>285</v>
       </c>
+      <c r="H176" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
@@ -3710,6 +3734,9 @@
       <c r="G177" t="s">
         <v>285</v>
       </c>
+      <c r="H177" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
@@ -3721,6 +3748,9 @@
       <c r="G178" t="s">
         <v>285</v>
       </c>
+      <c r="H178" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
@@ -3732,6 +3762,9 @@
       <c r="G179" t="s">
         <v>285</v>
       </c>
+      <c r="H179" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
@@ -3743,6 +3776,9 @@
       <c r="G180" t="s">
         <v>285</v>
       </c>
+      <c r="H180" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
@@ -3754,6 +3790,9 @@
       <c r="G181" t="s">
         <v>285</v>
       </c>
+      <c r="H181" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
@@ -3765,6 +3804,9 @@
       <c r="G182" t="s">
         <v>285</v>
       </c>
+      <c r="H182" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
@@ -3786,7 +3828,7 @@
         <v>376</v>
       </c>
       <c r="H183" t="s">
-        <v>376</v>
+        <v>285</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -3895,6 +3937,9 @@
       <c r="C190" t="s">
         <v>297</v>
       </c>
+      <c r="H190" t="s">
+        <v>285</v>
+      </c>
       <c r="I190">
         <v>1</v>
       </c>
@@ -3903,6 +3948,9 @@
       <c r="C191" t="s">
         <v>298</v>
       </c>
+      <c r="H191" t="s">
+        <v>285</v>
+      </c>
       <c r="I191">
         <v>1</v>
       </c>
@@ -3911,6 +3959,9 @@
       <c r="C192" t="s">
         <v>299</v>
       </c>
+      <c r="H192" t="s">
+        <v>285</v>
+      </c>
       <c r="I192">
         <v>1</v>
       </c>
@@ -3919,6 +3970,9 @@
       <c r="C193" t="s">
         <v>300</v>
       </c>
+      <c r="H193" t="s">
+        <v>285</v>
+      </c>
       <c r="I193">
         <v>1</v>
       </c>
@@ -3927,6 +3981,9 @@
       <c r="C194" t="s">
         <v>301</v>
       </c>
+      <c r="H194" t="s">
+        <v>285</v>
+      </c>
       <c r="I194">
         <v>1</v>
       </c>
@@ -3935,6 +3992,9 @@
       <c r="C195" t="s">
         <v>302</v>
       </c>
+      <c r="H195" t="s">
+        <v>285</v>
+      </c>
       <c r="I195">
         <v>1</v>
       </c>
@@ -3943,6 +4003,9 @@
       <c r="C196" t="s">
         <v>303</v>
       </c>
+      <c r="H196" t="s">
+        <v>285</v>
+      </c>
       <c r="I196">
         <v>1</v>
       </c>
@@ -3951,6 +4014,9 @@
       <c r="C197" t="s">
         <v>304</v>
       </c>
+      <c r="H197" t="s">
+        <v>285</v>
+      </c>
       <c r="I197">
         <v>1</v>
       </c>
@@ -3959,6 +4025,9 @@
       <c r="C198" t="s">
         <v>305</v>
       </c>
+      <c r="H198" t="s">
+        <v>285</v>
+      </c>
       <c r="I198">
         <v>1</v>
       </c>
@@ -3967,6 +4036,9 @@
       <c r="C199" t="s">
         <v>306</v>
       </c>
+      <c r="H199" t="s">
+        <v>285</v>
+      </c>
       <c r="I199">
         <v>1</v>
       </c>
@@ -3974,6 +4046,9 @@
     <row r="200" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C200" t="s">
         <v>307</v>
+      </c>
+      <c r="H200" t="s">
+        <v>285</v>
       </c>
       <c r="I200">
         <v>1</v>

</xml_diff>